<commit_message>
Issue #57, Make genre required with PBCore controlled vocabulary.
Includes:
* validation to make genre required;
* validation to ensure genre included in controlled vocabulary;
* user interface for form with autocomplete (modeled after the
  way the language field works, use Levenshtein distance to
  order matches);
* include authority and valueURI as attributes in MODS XML;
* allow manifest spreadsheet to override genre when doing
  bibliographic import;
* test suite upgrades (in particular spreadsheet fixtures);
</commit_message>
<xml_diff>
--- a/spec/fixtures/dropbox/example batch ingest/batch manifest with spaces.xlsx
+++ b/spec/fixtures/dropbox/example batch ingest/batch manifest with spaces.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t xml:space="preserve">Frances Dickens</t>
   </si>
@@ -55,6 +55,9 @@
     <t xml:space="preserve">Topical Subject</t>
   </si>
   <si>
+    <t xml:space="preserve">Genre</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dolorum</t>
   </si>
   <si>
@@ -80,6 +83,9 @@
   </si>
   <si>
     <t xml:space="preserve">Test subject</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bicycle</t>
   </si>
 </sst>
 </file>
@@ -192,23 +198,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4:J4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.9111111111111"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.7740740740741"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.9740740740741"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.4962962962963"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.2481481481481"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.8703703703704"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.07407407407407"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.3851851851852"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3037037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4592592592593"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.1814814814815"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.4444444444444"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.5555555555556"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.17407407407407"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -251,37 +257,43 @@
       <c r="J2" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="K2" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>2012</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>